<commit_message>
added google question soluton
</commit_message>
<xml_diff>
--- a/tracksheet.xlsx
+++ b/tracksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Important Stuff\CodingQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8DD025-5EC3-4188-845E-5F1B9EA53DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB2B7BF-65E4-4FC2-B5DD-610372E23701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D9598B2-69D8-457E-997A-7098C8D32A76}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="115">
   <si>
     <t>Date</t>
   </si>
@@ -368,12 +368,45 @@
   <si>
     <t xml:space="preserve">2 , brute force (TLE) , using deque -&gt; store index inside dequeu maintain the max element index  ,pop the elemnt from the queu which is either not in range or smaller then current element , to get the max value in current window we will append first elemtent of the deque </t>
   </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-left-leaves/</t>
+  </si>
+  <si>
+    <t>yes , only one time</t>
+  </si>
+  <si>
+    <t>1 , simple recusion with some special case</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-of-smaller-numbers-after-self/</t>
+  </si>
+  <si>
+    <t>bisect, binary search</t>
+  </si>
+  <si>
+    <t>yes, only once</t>
+  </si>
+  <si>
+    <t>1, triverse from end to start , maintain the list of visited elemnt in sorted order so that we can apply binary search to get the number lower then current element</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/discuss/interview-question/794840/Google-or-Software-Engineer-Internship-2021-or-Online-test-questions-(OA)</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>1, use concept of xor , instead of xoring each element multiple time calculate xor or all xor value and then calculate xor of every elemnt only once this will reduce time complexity from O(n**2) to O(n)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +433,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,7 +478,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -500,7 +546,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -823,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A007F2-951D-4EC1-9AD2-CBE187D69D00}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="E27" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1171,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44040</v>
       </c>
@@ -1384,7 +1445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44059</v>
       </c>
@@ -1442,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44059</v>
       </c>
@@ -1472,7 +1533,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44061</v>
       </c>
@@ -1682,8 +1743,93 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="12"/>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>44069</v>
+      </c>
+      <c r="B31" s="13">
+        <v>404</v>
+      </c>
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13">
+        <v>1</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>44069</v>
+      </c>
+      <c r="B32" s="16">
+        <v>315</v>
+      </c>
+      <c r="C32" s="16">
+        <v>1</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16">
+        <v>1</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1716,8 +1862,11 @@
     <hyperlink ref="D28" r:id="rId27" xr:uid="{CE26FC6E-914E-4874-93C4-1A4C909A1959}"/>
     <hyperlink ref="D29" r:id="rId28" xr:uid="{17D9D5BE-73A9-447F-9864-79D2D05FE3CB}"/>
     <hyperlink ref="D30" r:id="rId29" xr:uid="{F9DFFB50-5043-4395-878A-97A343D1C7B3}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{66C96818-B528-4CD4-88F2-B754DF3E3024}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{8D3E6301-D5F3-4831-836B-2F50473D0993}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{A74DCB3C-1B79-43CA-AC5D-EA6791D216E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kandane's Algorithm 1 Sept 2020
</commit_message>
<xml_diff>
--- a/tracksheet.xlsx
+++ b/tracksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Important Stuff\CodingQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D4DFB-6343-447D-B4C1-080C0D6FF199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95401143-2349-4BEE-BAA1-463B463D00B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1D9598B2-69D8-457E-997A-7098C8D32A76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1D9598B2-69D8-457E-997A-7098C8D32A76}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions Tracking Sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -472,10 +472,34 @@
     <t>https://www.geeksforgeeks.org/find-a-repeating-and-a-missing-number/</t>
   </si>
   <si>
-    <t>eq sum and product , xor method (need to implement)</t>
-  </si>
-  <si>
-    <t>equation. Xor</t>
+    <t xml:space="preserve">equation. Xor </t>
+  </si>
+  <si>
+    <t>eq sum and product , xor method : remember how to get a first set bit x &amp; ~(x-1)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hVl2b3bLzBw&amp;list=PLgUwDviBIf0rPG3Ictpu74YWBQ1CaBkm2&amp;index=4</t>
+  </si>
+  <si>
+    <t>using insertion sort, gap algorithm</t>
+  </si>
+  <si>
+    <t>yes definitely</t>
+  </si>
+  <si>
+    <t>Insertion sort: start from end compare element and insert elemnt such that sorting still maintained. Time complexity O(n*m) . Gap algorithm time complexity O(log2(n+m)*log(n+m))</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/</t>
+  </si>
+  <si>
+    <t>Kandane's algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">may be no </t>
+  </si>
+  <si>
+    <t>kandane's algorithm</t>
   </si>
 </sst>
 </file>
@@ -593,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -662,6 +686,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -989,7 +1031,7 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2102,10 +2144,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2161,7 @@
     <col min="7" max="7" width="23.85546875" style="20" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="20" customWidth="1"/>
     <col min="9" max="9" width="17.42578125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="35.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="61.85546875" style="20" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
@@ -2213,26 +2255,82 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>44074</v>
       </c>
       <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="22">
+        <v>1</v>
+      </c>
       <c r="D4" s="23" t="s">
         <v>137</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="I4" s="22">
+        <v>3</v>
+      </c>
       <c r="J4" s="22" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>44075</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>44075</v>
+      </c>
+      <c r="B6" s="28">
+        <v>53</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28">
+        <v>1</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2240,6 +2338,8 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{FDAB4594-DE12-4E39-A067-40D703C929AD}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{397E6175-C9A6-4842-8348-6E52819DA8B7}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{78CE589B-9262-4CC6-8F99-D3BA3FA8A4A4}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{29BC0F81-5AE4-406B-AD15-F87867705DCA}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{A52B3F96-63F6-4198-A013-E5D6A5800E69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
hard problem Reverse pair 10 Sept 2020
</commit_message>
<xml_diff>
--- a/tracksheet.xlsx
+++ b/tracksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Important Stuff\CodingQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36EC780-95AE-4134-B1F6-6DBD983D27E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD625FCA-3954-4A14-90C4-0DAFB0889FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1D9598B2-69D8-457E-997A-7098C8D32A76}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="192">
   <si>
     <t>Date</t>
   </si>
@@ -617,6 +617,22 @@
   </si>
   <si>
     <t>Boyer-Moore Voting Algorithm - enhanced</t>
+  </si>
+  <si>
+    <t>recursion , 2 D array , 1d array approach (Dynamic programming)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # number of path to reach a paticular cell is equal to the sum of
+ # number of unique path to react top and left cell  - we can optimize space using 1 d array also</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-pairs/</t>
+  </si>
+  <si>
+    <t>brute force</t>
+  </si>
+  <si>
+    <t>brute force (TLE)  , optimised modified inversion count (merge sort)</t>
   </si>
 </sst>
 </file>
@@ -2261,10 +2277,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,6 +2768,62 @@
         <v>181</v>
       </c>
     </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>44081</v>
+      </c>
+      <c r="B18" s="22">
+        <v>62</v>
+      </c>
+      <c r="C18" s="22">
+        <v>6</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
+        <v>3</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>44084</v>
+      </c>
+      <c r="B19" s="25">
+        <v>493</v>
+      </c>
+      <c r="C19" s="25">
+        <v>7</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25">
+        <v>3</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{FDAB4594-DE12-4E39-A067-40D703C929AD}"/>
@@ -2769,6 +2841,8 @@
     <hyperlink ref="D15" r:id="rId13" xr:uid="{7E836297-90F1-433E-A440-F0EF824D856F}"/>
     <hyperlink ref="D16" r:id="rId14" xr:uid="{A0B0EEC1-2F1E-4AA0-AC9E-AD15A65F95B5}"/>
     <hyperlink ref="D17" r:id="rId15" xr:uid="{700A667E-6CD7-4F51-B8DE-50E1B549E888}"/>
+    <hyperlink ref="D18" r:id="rId16" xr:uid="{4311EB59-FC68-4873-B270-DC52EA52E001}"/>
+    <hyperlink ref="D19" r:id="rId17" xr:uid="{B1DC559A-5FC1-42CD-8AC2-76C41B948E79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>